<commit_message>
ASK-41 Fix last remaining benchmark
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmarktest_traject INNW 22-1.xlsx
+++ b/benchmarktests/testdefinitions/Benchmarktest_traject INNW 22-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD8C433-4B49-4A11-9530-521A8C30C58D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF1BF83-9527-431D-9E55-709B7D504DA9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7665" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="2" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="0" yWindow="510" windowWidth="28800" windowHeight="15435" tabRatio="653" firstSheet="1" activeTab="2" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="174">
   <si>
     <t>Vaknaam</t>
   </si>
@@ -568,9 +568,6 @@
   <si>
     <t>Gecombineerd (tussentijds)</t>
   </si>
-  <si>
-    <t>0.00023947736549434495</t>
-  </si>
 </sst>
 </file>
 
@@ -846,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -926,6 +923,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2593,7 +2602,7 @@
   <dimension ref="B1:L117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E82"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,7 +2663,7 @@
         <v>+I</v>
       </c>
       <c r="F3" s="4" t="str">
-        <f t="array" ref="F3">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B3,C3),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F3">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B3,C3),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G3" s="4" t="str">
@@ -2698,7 +2707,7 @@
         <v>+I</v>
       </c>
       <c r="F4" s="9" t="str">
-        <f t="array" ref="F4">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B4,C4),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F4">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B4,C4),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G4" s="9" t="str">
@@ -2731,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="9">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="D5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -2742,7 +2751,7 @@
         <v>+I</v>
       </c>
       <c r="F5" s="9" t="str">
-        <f t="array" ref="F5">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B5,C5),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F5">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B5,C5),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G5" s="9" t="str">
@@ -2772,10 +2781,10 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="C6" s="9">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="D6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -2786,7 +2795,7 @@
         <v>+I</v>
       </c>
       <c r="F6" s="9" t="str">
-        <f t="array" ref="F6">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B6,C6),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F6">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B6,C6),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G6" s="9" t="str">
@@ -2803,23 +2812,23 @@
       </c>
       <c r="J6" s="9" t="str">
         <f t="array" ref="J6">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B6,C6),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K6" s="9" t="str">
         <f t="array" ref="K6">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B6,C6),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L6" s="12" t="str">
         <f t="array" ref="L6">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B6,C6),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="C7" s="9">
-        <v>1.41</v>
+        <v>1.7</v>
       </c>
       <c r="D7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -2830,7 +2839,7 @@
         <v>+I</v>
       </c>
       <c r="F7" s="9" t="str">
-        <f t="array" ref="F7">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B7,C7),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F7">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B7,C7),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G7" s="9" t="str">
@@ -2847,23 +2856,23 @@
       </c>
       <c r="J7" s="9" t="str">
         <f t="array" ref="J7">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B7,C7),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K7" s="9" t="str">
         <f t="array" ref="K7">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B7,C7),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L7" s="12" t="str">
         <f t="array" ref="L7">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B7,C7),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
-        <v>1.41</v>
+        <v>1.7</v>
       </c>
       <c r="C8" s="9">
-        <v>1.7</v>
+        <v>1.71</v>
       </c>
       <c r="D8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -2874,12 +2883,12 @@
         <v>+I</v>
       </c>
       <c r="F8" s="9" t="str">
-        <f t="array" ref="F8">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B8,C8),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F8">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B8,C8),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G8" s="9" t="str">
         <f t="array" ref="G8">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B8,C8),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H8" s="9" t="str">
         <f t="array" ref="H8">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -2891,23 +2900,23 @@
       </c>
       <c r="J8" s="9" t="str">
         <f t="array" ref="J8">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B8,C8),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K8" s="9" t="str">
         <f t="array" ref="K8">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B8,C8),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L8" s="12" t="str">
         <f t="array" ref="L8">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B8,C8),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
-        <v>1.7</v>
+        <v>1.71</v>
       </c>
       <c r="C9" s="9">
-        <v>1.71</v>
+        <v>2.5</v>
       </c>
       <c r="D9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -2918,7 +2927,7 @@
         <v>+I</v>
       </c>
       <c r="F9" s="9" t="str">
-        <f t="array" ref="F9">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B9,C9),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F9">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B9,C9),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G9" s="9" t="str">
@@ -2935,39 +2944,39 @@
       </c>
       <c r="J9" s="9" t="str">
         <f t="array" ref="J9">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B9,C9),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K9" s="9" t="str">
         <f t="array" ref="K9">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B9,C9),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L9" s="12" t="str">
         <f t="array" ref="L9">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B9,C9),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
-        <v>1.71</v>
+        <v>2.5</v>
       </c>
       <c r="C10" s="9">
-        <v>2.5</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D10" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="E10" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="F10" s="9" t="str">
-        <f t="array" ref="F10">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B10,C10),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F10">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B10,C10),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+0</v>
       </c>
       <c r="G10" s="9" t="str">
         <f t="array" ref="G10">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B10,C10),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H10" s="9" t="str">
         <f t="array" ref="H10">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -2979,23 +2988,23 @@
       </c>
       <c r="J10" s="9" t="str">
         <f t="array" ref="J10">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B10,C10),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K10" s="9" t="str">
         <f t="array" ref="K10">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B10,C10),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L10" s="12" t="str">
         <f t="array" ref="L10">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B10,C10),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
-        <v>2.5</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="C11" s="9">
-        <v>2.5099999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="D11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3006,7 +3015,7 @@
         <v>+0</v>
       </c>
       <c r="F11" s="9" t="str">
-        <f t="array" ref="F11">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B11,C11),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F11">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B11,C11),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+0</v>
       </c>
       <c r="G11" s="9" t="str">
@@ -3023,23 +3032,23 @@
       </c>
       <c r="J11" s="9" t="str">
         <f t="array" ref="J11">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B11,C11),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K11" s="9" t="str">
         <f t="array" ref="K11">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B11,C11),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L11" s="12" t="str">
         <f t="array" ref="L11">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B11,C11),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
-        <v>2.5099999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="C12" s="9">
-        <v>2.8</v>
+        <v>2.81</v>
       </c>
       <c r="D12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3050,7 +3059,7 @@
         <v>+0</v>
       </c>
       <c r="F12" s="9" t="str">
-        <f t="array" ref="F12">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B12,C12),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F12">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B12,C12),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+0</v>
       </c>
       <c r="G12" s="9" t="str">
@@ -3067,23 +3076,23 @@
       </c>
       <c r="J12" s="9" t="str">
         <f t="array" ref="J12">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B12,C12),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K12" s="9" t="str">
         <f t="array" ref="K12">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B12,C12),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L12" s="12" t="str">
         <f t="array" ref="L12">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B12,C12),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
-        <v>2.8</v>
+        <v>2.81</v>
       </c>
       <c r="C13" s="9">
-        <v>2.81</v>
+        <v>3.0999999999999996</v>
       </c>
       <c r="D13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3094,7 +3103,7 @@
         <v>+0</v>
       </c>
       <c r="F13" s="9" t="str">
-        <f t="array" ref="F13">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B13,C13),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F13">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B13,C13),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+0</v>
       </c>
       <c r="G13" s="9" t="str">
@@ -3111,23 +3120,23 @@
       </c>
       <c r="J13" s="9" t="str">
         <f t="array" ref="J13">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B13,C13),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K13" s="9" t="str">
         <f t="array" ref="K13">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B13,C13),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L13" s="12" t="str">
         <f t="array" ref="L13">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B13,C13),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
-        <v>2.81</v>
+        <v>3.0999999999999996</v>
       </c>
       <c r="C14" s="9">
-        <v>3.0999999999999996</v>
+        <v>4.2000000000000011</v>
       </c>
       <c r="D14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3138,12 +3147,12 @@
         <v>+0</v>
       </c>
       <c r="F14" s="9" t="str">
-        <f t="array" ref="F14">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B14,C14),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F14">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B14,C14),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+0</v>
       </c>
       <c r="G14" s="9" t="str">
         <f t="array" ref="G14">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B14,C14),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+I</v>
       </c>
       <c r="H14" s="9" t="str">
         <f t="array" ref="H14">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3168,26 +3177,26 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
-        <v>3.0999999999999996</v>
+        <v>4.2000000000000011</v>
       </c>
       <c r="C15" s="9">
-        <v>3.8</v>
+        <v>4.5500000000000007</v>
       </c>
       <c r="D15" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="E15" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="F15" s="9" t="str">
-        <f t="array" ref="F15">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B15,C15),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+0</v>
+        <f t="array" ref="F15">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B15,C15),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G15" s="9" t="str">
         <f t="array" ref="G15">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B15,C15),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+I</v>
+        <v>+III</v>
       </c>
       <c r="H15" s="9" t="str">
         <f t="array" ref="H15">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B15,C15),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3212,26 +3221,26 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
-        <v>3.8</v>
+        <v>4.5500000000000007</v>
       </c>
       <c r="C16" s="9">
-        <v>4.2000000000000011</v>
+        <v>5.6</v>
       </c>
       <c r="D16" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+0</v>
+        <v>+I</v>
       </c>
       <c r="F16" s="9" t="str">
-        <f t="array" ref="F16">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B16,C16),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+0</v>
+        <f t="array" ref="F16">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B16,C16),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G16" s="9" t="str">
         <f t="array" ref="G16">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B16,C16),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+I</v>
+        <v>+III</v>
       </c>
       <c r="H16" s="9" t="str">
         <f t="array" ref="H16">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B16,C16),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3256,10 +3265,10 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
-        <v>4.2000000000000011</v>
+        <v>5.6</v>
       </c>
       <c r="C17" s="9">
-        <v>4.5500000000000007</v>
+        <v>5.9</v>
       </c>
       <c r="D17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3270,7 +3279,7 @@
         <v>+I</v>
       </c>
       <c r="F17" s="9" t="str">
-        <f t="array" ref="F17">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B17,C17),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F17">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B17,C17),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G17" s="9" t="str">
@@ -3300,10 +3309,10 @@
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
-        <v>4.5500000000000007</v>
+        <v>5.9</v>
       </c>
       <c r="C18" s="9">
-        <v>5.4</v>
+        <v>5.91</v>
       </c>
       <c r="D18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3314,7 +3323,7 @@
         <v>+I</v>
       </c>
       <c r="F18" s="9" t="str">
-        <f t="array" ref="F18">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B18,C18),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F18">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B18,C18),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G18" s="9" t="str">
@@ -3331,23 +3340,23 @@
       </c>
       <c r="J18" s="9" t="str">
         <f t="array" ref="J18">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B18,C18),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K18" s="9" t="str">
         <f t="array" ref="K18">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B18,C18),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L18" s="12" t="str">
         <f t="array" ref="L18">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B18,C18),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
-        <v>5.4</v>
+        <v>5.91</v>
       </c>
       <c r="C19" s="9">
-        <v>5.6</v>
+        <v>6.2000000000000011</v>
       </c>
       <c r="D19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3358,7 +3367,7 @@
         <v>+I</v>
       </c>
       <c r="F19" s="9" t="str">
-        <f t="array" ref="F19">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B19,C19),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F19">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B19,C19),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G19" s="9" t="str">
@@ -3388,22 +3397,22 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
-        <v>5.6</v>
+        <v>6.2000000000000011</v>
       </c>
       <c r="C20" s="9">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="D20" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E20" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F20" s="9" t="str">
-        <f t="array" ref="F20">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B20,C20),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F20">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B20,C20),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G20" s="9" t="str">
         <f t="array" ref="G20">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B20,C20),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -3432,22 +3441,22 @@
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="C21" s="9">
-        <v>5.91</v>
+        <v>6.71</v>
       </c>
       <c r="D21" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E21" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F21" s="9" t="str">
-        <f t="array" ref="F21">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B21,C21),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F21">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B21,C21),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G21" s="9" t="str">
         <f t="array" ref="G21">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B21,C21),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -3476,22 +3485,22 @@
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
-        <v>5.91</v>
+        <v>6.71</v>
       </c>
       <c r="C22" s="9">
-        <v>6.2000000000000011</v>
+        <v>7.1</v>
       </c>
       <c r="D22" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E22" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F22" s="9" t="str">
-        <f t="array" ref="F22">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B22,C22),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F22">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B22,C22),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G22" s="9" t="str">
         <f t="array" ref="G22">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B22,C22),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -3520,10 +3529,10 @@
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
-        <v>6.2000000000000011</v>
+        <v>7.1</v>
       </c>
       <c r="C23" s="9">
-        <v>6.7</v>
+        <v>7.11</v>
       </c>
       <c r="D23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3534,7 +3543,7 @@
         <v>+II</v>
       </c>
       <c r="F23" s="9" t="str">
-        <f t="array" ref="F23">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B23,C23),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F23">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B23,C23),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G23" s="9" t="str">
@@ -3551,23 +3560,23 @@
       </c>
       <c r="J23" s="9" t="str">
         <f t="array" ref="J23">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B23,C23),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K23" s="9" t="str">
         <f t="array" ref="K23">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B23,C23),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L23" s="12" t="str">
         <f t="array" ref="L23">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B23,C23),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
-        <v>6.7</v>
+        <v>7.11</v>
       </c>
       <c r="C24" s="9">
-        <v>6.71</v>
+        <v>7.35</v>
       </c>
       <c r="D24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3578,7 +3587,7 @@
         <v>+II</v>
       </c>
       <c r="F24" s="9" t="str">
-        <f t="array" ref="F24">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B24,C24),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F24">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B24,C24),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G24" s="9" t="str">
@@ -3595,39 +3604,39 @@
       </c>
       <c r="J24" s="9" t="str">
         <f t="array" ref="J24">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B24,C24),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K24" s="9" t="str">
         <f t="array" ref="K24">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B24,C24),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L24" s="12" t="str">
         <f t="array" ref="L24">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B24,C24),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
-        <v>6.71</v>
+        <v>7.35</v>
       </c>
       <c r="C25" s="9">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="D25" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="E25" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="F25" s="9" t="str">
-        <f t="array" ref="F25">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B25,C25),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F25">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B25,C25),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G25" s="9" t="str">
         <f t="array" ref="G25">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B25,C25),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H25" s="9" t="str">
         <f t="array" ref="H25">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B25,C25),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3652,26 +3661,26 @@
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
-        <v>7.1</v>
+        <v>7.7</v>
       </c>
       <c r="C26" s="9">
-        <v>7.11</v>
+        <v>7.71</v>
       </c>
       <c r="D26" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="E26" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="F26" s="9" t="str">
-        <f t="array" ref="F26">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B26,C26),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F26">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B26,C26),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G26" s="9" t="str">
         <f t="array" ref="G26">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B26,C26),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H26" s="9" t="str">
         <f t="array" ref="H26">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B26,C26),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3696,26 +3705,26 @@
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
-        <v>7.11</v>
+        <v>7.71</v>
       </c>
       <c r="C27" s="9">
-        <v>7.35</v>
+        <v>8.25</v>
       </c>
       <c r="D27" s="23" t="str">
         <f t="shared" si="0"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="E27" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="F27" s="9" t="str">
-        <f t="array" ref="F27">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B27,C27),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F27">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B27,C27),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G27" s="9" t="str">
         <f t="array" ref="G27">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B27,C27),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+II</v>
       </c>
       <c r="H27" s="9" t="str">
         <f t="array" ref="H27">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B27,C27),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3740,10 +3749,10 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
-        <v>7.35</v>
+        <v>8.25</v>
       </c>
       <c r="C28" s="9">
-        <v>7.7</v>
+        <v>8.26</v>
       </c>
       <c r="D28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3754,7 +3763,7 @@
         <v>+I</v>
       </c>
       <c r="F28" s="9" t="str">
-        <f t="array" ref="F28">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B28,C28),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F28">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B28,C28),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G28" s="9" t="str">
@@ -3771,23 +3780,23 @@
       </c>
       <c r="J28" s="9" t="str">
         <f t="array" ref="J28">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B28,C28),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K28" s="9" t="str">
         <f t="array" ref="K28">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B28,C28),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L28" s="12" t="str">
         <f t="array" ref="L28">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B28,C28),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
-        <v>7.7</v>
+        <v>8.26</v>
       </c>
       <c r="C29" s="9">
-        <v>7.71</v>
+        <v>9.1</v>
       </c>
       <c r="D29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3798,7 +3807,7 @@
         <v>+I</v>
       </c>
       <c r="F29" s="9" t="str">
-        <f t="array" ref="F29">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B29,C29),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F29">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B29,C29),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G29" s="9" t="str">
@@ -3815,23 +3824,23 @@
       </c>
       <c r="J29" s="9" t="str">
         <f t="array" ref="J29">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B29,C29),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K29" s="9" t="str">
         <f t="array" ref="K29">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B29,C29),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L29" s="12" t="str">
         <f t="array" ref="L29">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B29,C29),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
-        <v>7.71</v>
+        <v>9.1</v>
       </c>
       <c r="C30" s="9">
-        <v>8.25</v>
+        <v>9.4</v>
       </c>
       <c r="D30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3842,7 +3851,7 @@
         <v>+I</v>
       </c>
       <c r="F30" s="9" t="str">
-        <f t="array" ref="F30">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B30,C30),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F30">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B30,C30),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G30" s="9" t="str">
@@ -3872,10 +3881,10 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
-        <v>8.25</v>
+        <v>9.4</v>
       </c>
       <c r="C31" s="9">
-        <v>8.26</v>
+        <v>10</v>
       </c>
       <c r="D31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3886,12 +3895,12 @@
         <v>+I</v>
       </c>
       <c r="F31" s="9" t="str">
-        <f t="array" ref="F31">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B31,C31),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F31">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B31,C31),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G31" s="9" t="str">
         <f t="array" ref="G31">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B31,C31),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="H31" s="9" t="str">
         <f t="array" ref="H31">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B31,C31),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3903,23 +3912,23 @@
       </c>
       <c r="J31" s="9" t="str">
         <f t="array" ref="J31">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B31,C31),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K31" s="9" t="str">
         <f t="array" ref="K31">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B31,C31),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L31" s="12" t="str">
         <f t="array" ref="L31">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B31,C31),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
-        <v>8.26</v>
+        <v>10</v>
       </c>
       <c r="C32" s="9">
-        <v>9.1</v>
+        <v>10.01</v>
       </c>
       <c r="D32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3930,12 +3939,12 @@
         <v>+I</v>
       </c>
       <c r="F32" s="9" t="str">
-        <f t="array" ref="F32">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B32,C32),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F32">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B32,C32),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G32" s="9" t="str">
         <f t="array" ref="G32">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B32,C32),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="H32" s="9" t="str">
         <f t="array" ref="H32">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B32,C32),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -3947,23 +3956,23 @@
       </c>
       <c r="J32" s="9" t="str">
         <f t="array" ref="J32">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B32,C32),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="K32" s="9" t="str">
         <f t="array" ref="K32">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B32,C32),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="L32" s="12" t="str">
         <f t="array" ref="L32">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B32,C32),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8">
-        <v>9.1</v>
+        <v>10.01</v>
       </c>
       <c r="C33" s="9">
-        <v>9.4</v>
+        <v>10.1</v>
       </c>
       <c r="D33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -3974,12 +3983,12 @@
         <v>+I</v>
       </c>
       <c r="F33" s="9" t="str">
-        <f t="array" ref="F33">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B33,C33),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F33">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B33,C33),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G33" s="9" t="str">
         <f t="array" ref="G33">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B33,C33),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="H33" s="9" t="str">
         <f t="array" ref="H33">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B33,C33),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4004,10 +4013,10 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="8">
-        <v>9.4</v>
+        <v>10.1</v>
       </c>
       <c r="C34" s="9">
-        <v>10</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D34" s="23" t="str">
         <f t="shared" si="0"/>
@@ -4018,7 +4027,7 @@
         <v>+I</v>
       </c>
       <c r="F34" s="9" t="str">
-        <f t="array" ref="F34">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B34,C34),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F34">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B34,C34),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G34" s="9" t="str">
@@ -4048,10 +4057,10 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
-        <v>10</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="C35" s="9">
-        <v>10.01</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="D35" s="23" t="str">
         <f t="shared" ref="D35:D66" si="2">IF(COUNTIF(F35:L35,"D")&gt;0,"D",IF(COUNTIF(F35:L35,"-III")&gt;0,"-III",IF(COUNTIF(F35:L35,"-II")&gt;0,"-II",IF(COUNTIF(F35:L35,"-I")&gt;0,"-I",IF(COUNTIF(F35:L35,"+0")&gt;0,"+0",IF(COUNTIF(F35:L35,"+I")&gt;0,"+I",IF(COUNTIF(F35:L35,"+II")&gt;0,"+II",IF(COUNTIF(F35:L35,"+III")&gt;0,"+III",IF(COUNTIF(F35:L35,"ND")&gt;0,"ND","NR")))))))))</f>
@@ -4062,7 +4071,7 @@
         <v>+I</v>
       </c>
       <c r="F35" s="9" t="str">
-        <f t="array" ref="F35">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B35,C35),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F35">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B35,C35),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G35" s="9" t="str">
@@ -4092,10 +4101,10 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
-        <v>10.01</v>
+        <v>10.210000000000001</v>
       </c>
       <c r="C36" s="9">
-        <v>10.1</v>
+        <v>10.55</v>
       </c>
       <c r="D36" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4106,7 +4115,7 @@
         <v>+I</v>
       </c>
       <c r="F36" s="9" t="str">
-        <f t="array" ref="F36">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B36,C36),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F36">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B36,C36),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G36" s="9" t="str">
@@ -4136,10 +4145,10 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
-        <v>10.1</v>
+        <v>10.55</v>
       </c>
       <c r="C37" s="9">
-        <v>10.199999999999999</v>
+        <v>10.56</v>
       </c>
       <c r="D37" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4150,7 +4159,7 @@
         <v>+I</v>
       </c>
       <c r="F37" s="9" t="str">
-        <f t="array" ref="F37">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B37,C37),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F37">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B37,C37),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G37" s="9" t="str">
@@ -4167,23 +4176,23 @@
       </c>
       <c r="J37" s="9" t="str">
         <f t="array" ref="J37">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B37,C37),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="K37" s="9" t="str">
         <f t="array" ref="K37">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B37,C37),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L37" s="12" t="str">
         <f t="array" ref="L37">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B37,C37),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
-        <v>10.199999999999999</v>
+        <v>10.56</v>
       </c>
       <c r="C38" s="9">
-        <v>10.210000000000001</v>
+        <v>10.6</v>
       </c>
       <c r="D38" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4194,7 +4203,7 @@
         <v>+I</v>
       </c>
       <c r="F38" s="9" t="str">
-        <f t="array" ref="F38">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B38,C38),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F38">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B38,C38),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G38" s="9" t="str">
@@ -4211,23 +4220,23 @@
       </c>
       <c r="J38" s="9" t="str">
         <f t="array" ref="J38">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B38,C38),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
       <c r="K38" s="9" t="str">
         <f t="array" ref="K38">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B38,C38),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
       <c r="L38" s="12" t="str">
         <f t="array" ref="L38">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B38,C38),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="8">
-        <v>10.210000000000001</v>
+        <v>10.6</v>
       </c>
       <c r="C39" s="9">
-        <v>10.55</v>
+        <v>11</v>
       </c>
       <c r="D39" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4238,12 +4247,12 @@
         <v>+I</v>
       </c>
       <c r="F39" s="9" t="str">
-        <f t="array" ref="F39">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B39,C39),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F39">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B39,C39),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G39" s="9" t="str">
         <f t="array" ref="G39">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B39,C39),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="H39" s="9" t="str">
         <f t="array" ref="H39">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B39,C39),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4268,10 +4277,10 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
-        <v>10.55</v>
+        <v>11</v>
       </c>
       <c r="C40" s="9">
-        <v>10.56</v>
+        <v>11.01</v>
       </c>
       <c r="D40" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4282,12 +4291,12 @@
         <v>+I</v>
       </c>
       <c r="F40" s="9" t="str">
-        <f t="array" ref="F40">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B40,C40),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F40">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B40,C40),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G40" s="9" t="str">
         <f t="array" ref="G40">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B40,C40),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="H40" s="9" t="str">
         <f t="array" ref="H40">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B40,C40),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4299,7 +4308,7 @@
       </c>
       <c r="J40" s="9" t="str">
         <f t="array" ref="J40">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B40,C40),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="K40" s="9" t="str">
         <f t="array" ref="K40">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B40,C40),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
@@ -4307,15 +4316,15 @@
       </c>
       <c r="L40" s="12" t="str">
         <f t="array" ref="L40">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B40,C40),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="8">
-        <v>10.56</v>
+        <v>11.01</v>
       </c>
       <c r="C41" s="9">
-        <v>10.6</v>
+        <v>11.799999999999999</v>
       </c>
       <c r="D41" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4326,12 +4335,12 @@
         <v>+I</v>
       </c>
       <c r="F41" s="9" t="str">
-        <f t="array" ref="F41">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B41,C41),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F41">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B41,C41),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G41" s="9" t="str">
         <f t="array" ref="G41">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B41,C41),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="H41" s="9" t="str">
         <f t="array" ref="H41">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B41,C41),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4356,10 +4365,10 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
-        <v>10.6</v>
+        <v>11.799999999999999</v>
       </c>
       <c r="C42" s="9">
-        <v>11</v>
+        <v>11.81</v>
       </c>
       <c r="D42" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4370,7 +4379,7 @@
         <v>+I</v>
       </c>
       <c r="F42" s="9" t="str">
-        <f t="array" ref="F42">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B42,C42),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F42">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B42,C42),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G42" s="9" t="str">
@@ -4387,23 +4396,23 @@
       </c>
       <c r="J42" s="9" t="str">
         <f t="array" ref="J42">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B42,C42),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K42" s="9" t="str">
         <f t="array" ref="K42">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B42,C42),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L42" s="12" t="str">
         <f t="array" ref="L42">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B42,C42),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
-        <v>11</v>
+        <v>11.81</v>
       </c>
       <c r="C43" s="9">
-        <v>11.01</v>
+        <v>12.200000000000001</v>
       </c>
       <c r="D43" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4414,7 +4423,7 @@
         <v>+I</v>
       </c>
       <c r="F43" s="9" t="str">
-        <f t="array" ref="F43">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B43,C43),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F43">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B43,C43),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+I</v>
       </c>
       <c r="G43" s="9" t="str">
@@ -4431,35 +4440,35 @@
       </c>
       <c r="J43" s="9" t="str">
         <f t="array" ref="J43">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B43,C43),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K43" s="9" t="str">
         <f t="array" ref="K43">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B43,C43),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L43" s="12" t="str">
         <f t="array" ref="L43">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B43,C43),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
-        <v>11.01</v>
+        <v>12.200000000000001</v>
       </c>
       <c r="C44" s="9">
-        <v>11.4</v>
+        <v>12.500000000000002</v>
       </c>
       <c r="D44" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E44" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F44" s="9" t="str">
-        <f t="array" ref="F44">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B44,C44),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F44">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B44,C44),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G44" s="9" t="str">
         <f t="array" ref="G44">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B44,C44),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -4488,26 +4497,26 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
-        <v>11.4</v>
+        <v>12.500000000000002</v>
       </c>
       <c r="C45" s="9">
-        <v>11.799999999999999</v>
+        <v>13</v>
       </c>
       <c r="D45" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F45" s="9" t="str">
-        <f t="array" ref="F45">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B45,C45),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F45">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B45,C45),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G45" s="9" t="str">
         <f t="array" ref="G45">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B45,C45),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H45" s="9" t="str">
         <f t="array" ref="H45">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B45,C45),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4532,10 +4541,10 @@
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
-        <v>11.799999999999999</v>
+        <v>13</v>
       </c>
       <c r="C46" s="9">
-        <v>11.81</v>
+        <v>13.01</v>
       </c>
       <c r="D46" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4546,12 +4555,12 @@
         <v>+I</v>
       </c>
       <c r="F46" s="9" t="str">
-        <f t="array" ref="F46">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B46,C46),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F46">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B46,C46),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G46" s="9" t="str">
         <f t="array" ref="G46">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B46,C46),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H46" s="9" t="str">
         <f t="array" ref="H46">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B46,C46),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4563,39 +4572,39 @@
       </c>
       <c r="J46" s="9" t="str">
         <f t="array" ref="J46">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B46,C46),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="K46" s="9" t="str">
         <f t="array" ref="K46">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B46,C46),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="L46" s="12" t="str">
         <f t="array" ref="L46">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B46,C46),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>+I</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
-        <v>11.81</v>
+        <v>13.01</v>
       </c>
       <c r="C47" s="9">
-        <v>12.1</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="D47" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F47" s="9" t="str">
-        <f t="array" ref="F47">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B47,C47),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F47">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B47,C47),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G47" s="9" t="str">
         <f t="array" ref="G47">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B47,C47),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H47" s="9" t="str">
         <f t="array" ref="H47">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B47,C47),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4620,26 +4629,26 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
-        <v>12.1</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="C48" s="9">
-        <v>12.200000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="D48" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="E48" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="F48" s="9" t="str">
-        <f t="array" ref="F48">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B48,C48),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
+        <f t="array" ref="F48">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B48,C48),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+III</v>
       </c>
       <c r="G48" s="9" t="str">
         <f t="array" ref="G48">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B48,C48),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H48" s="9" t="str">
         <f t="array" ref="H48">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B48,C48),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4664,10 +4673,10 @@
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
-        <v>12.200000000000001</v>
+        <v>13.4</v>
       </c>
       <c r="C49" s="9">
-        <v>12.500000000000002</v>
+        <v>13.41</v>
       </c>
       <c r="D49" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4678,12 +4687,12 @@
         <v>+II</v>
       </c>
       <c r="F49" s="9" t="str">
-        <f t="array" ref="F49">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B49,C49),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F49">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B49,C49),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G49" s="9" t="str">
         <f t="array" ref="G49">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B49,C49),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+II</v>
+        <v>+III</v>
       </c>
       <c r="H49" s="9" t="str">
         <f t="array" ref="H49">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B49,C49),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4695,23 +4704,23 @@
       </c>
       <c r="J49" s="9" t="str">
         <f t="array" ref="J49">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B49,C49),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K49" s="9" t="str">
         <f t="array" ref="K49">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B49,C49),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L49" s="12" t="str">
         <f t="array" ref="L49">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B49,C49),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
-        <v>12.500000000000002</v>
+        <v>13.41</v>
       </c>
       <c r="C50" s="9">
-        <v>12.7</v>
+        <v>13.9</v>
       </c>
       <c r="D50" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4722,7 +4731,7 @@
         <v>+II</v>
       </c>
       <c r="F50" s="9" t="str">
-        <f t="array" ref="F50">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B50,C50),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F50">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B50,C50),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G50" s="9" t="str">
@@ -4752,21 +4761,21 @@
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
-        <v>12.7</v>
+        <v>13.9</v>
       </c>
       <c r="C51" s="9">
-        <v>12.799999999999999</v>
+        <v>13.91</v>
       </c>
       <c r="D51" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="E51" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+I</v>
       </c>
       <c r="F51" s="9" t="str">
-        <f t="array" ref="F51">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B51,C51),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F51">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B51,C51),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G51" s="9" t="str">
@@ -4783,23 +4792,23 @@
       </c>
       <c r="J51" s="9" t="str">
         <f t="array" ref="J51">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B51,C51),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="K51" s="9" t="str">
         <f t="array" ref="K51">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B51,C51),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
       <c r="L51" s="12" t="str">
         <f t="array" ref="L51">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B51,C51),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+I</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
-        <v>12.799999999999999</v>
+        <v>13.91</v>
       </c>
       <c r="C52" s="9">
-        <v>13</v>
+        <v>14.2</v>
       </c>
       <c r="D52" s="23" t="str">
         <f t="shared" si="2"/>
@@ -4810,7 +4819,7 @@
         <v>+II</v>
       </c>
       <c r="F52" s="9" t="str">
-        <f t="array" ref="F52">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B52,C52),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F52">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B52,C52),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G52" s="9" t="str">
@@ -4840,26 +4849,26 @@
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="8">
-        <v>13</v>
+        <v>14.2</v>
       </c>
       <c r="C53" s="9">
-        <v>13.01</v>
+        <v>14.21</v>
       </c>
       <c r="D53" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>-II</v>
       </c>
       <c r="E53" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>-II</v>
       </c>
       <c r="F53" s="9" t="str">
-        <f t="array" ref="F53">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B53,C53),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F53">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B53,C53),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G53" s="9" t="str">
         <f t="array" ref="G53">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B53,C53),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>-II</v>
       </c>
       <c r="H53" s="9" t="str">
         <f t="array" ref="H53">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B53,C53),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4871,39 +4880,39 @@
       </c>
       <c r="J53" s="9" t="str">
         <f t="array" ref="J53">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B53,C53),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="K53" s="9" t="str">
         <f t="array" ref="K53">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B53,C53),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
       <c r="L53" s="12" t="str">
         <f t="array" ref="L53">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B53,C53),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+I</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="8">
-        <v>13.01</v>
+        <v>14.21</v>
       </c>
       <c r="C54" s="9">
-        <v>13.200000000000001</v>
+        <v>14.4</v>
       </c>
       <c r="D54" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="E54" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="F54" s="9" t="str">
-        <f t="array" ref="F54">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B54,C54),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F54">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B54,C54),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G54" s="9" t="str">
         <f t="array" ref="G54">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B54,C54),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>-II</v>
       </c>
       <c r="H54" s="9" t="str">
         <f t="array" ref="H54">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B54,C54),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4928,26 +4937,26 @@
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="8">
-        <v>13.200000000000001</v>
+        <v>14.4</v>
       </c>
       <c r="C55" s="9">
-        <v>13.4</v>
+        <v>14.799999999999999</v>
       </c>
       <c r="D55" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="E55" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>-II</v>
       </c>
       <c r="F55" s="9" t="str">
-        <f t="array" ref="F55">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B55,C55),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F55">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B55,C55),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G55" s="9" t="str">
         <f t="array" ref="G55">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B55,C55),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>-II</v>
       </c>
       <c r="H55" s="9" t="str">
         <f t="array" ref="H55">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B55,C55),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -4972,26 +4981,26 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="8">
-        <v>13.4</v>
+        <v>14.799999999999999</v>
       </c>
       <c r="C56" s="9">
-        <v>13.41</v>
+        <v>15</v>
       </c>
       <c r="D56" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="E56" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="F56" s="9" t="str">
-        <f t="array" ref="F56">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B56,C56),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F56">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B56,C56),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G56" s="9" t="str">
         <f t="array" ref="G56">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B56,C56),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+0</v>
       </c>
       <c r="H56" s="9" t="str">
         <f t="array" ref="H56">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B56,C56),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5003,39 +5012,39 @@
       </c>
       <c r="J56" s="9" t="str">
         <f t="array" ref="J56">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B56,C56),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K56" s="9" t="str">
         <f t="array" ref="K56">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B56,C56),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L56" s="12" t="str">
         <f t="array" ref="L56">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B56,C56),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="8">
-        <v>13.41</v>
+        <v>15</v>
       </c>
       <c r="C57" s="9">
-        <v>13.9</v>
+        <v>15.01</v>
       </c>
       <c r="D57" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="E57" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="F57" s="9" t="str">
-        <f t="array" ref="F57">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B57,C57),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F57">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B57,C57),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G57" s="9" t="str">
         <f t="array" ref="G57">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B57,C57),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+0</v>
       </c>
       <c r="H57" s="9" t="str">
         <f t="array" ref="H57">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B57,C57),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5047,39 +5056,39 @@
       </c>
       <c r="J57" s="9" t="str">
         <f t="array" ref="J57">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B57,C57),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K57" s="9" t="str">
         <f t="array" ref="K57">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B57,C57),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L57" s="12" t="str">
         <f t="array" ref="L57">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B57,C57),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="8">
-        <v>13.9</v>
+        <v>15.01</v>
       </c>
       <c r="C58" s="9">
-        <v>13.91</v>
+        <v>15.7</v>
       </c>
       <c r="D58" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="E58" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+I</v>
+        <v>+0</v>
       </c>
       <c r="F58" s="9" t="str">
-        <f t="array" ref="F58">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B58,C58),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F58">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B58,C58),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G58" s="9" t="str">
         <f t="array" ref="G58">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B58,C58),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+0</v>
       </c>
       <c r="H58" s="9" t="str">
         <f t="array" ref="H58">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B58,C58),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5091,39 +5100,39 @@
       </c>
       <c r="J58" s="9" t="str">
         <f t="array" ref="J58">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B58,C58),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
       <c r="K58" s="9" t="str">
         <f t="array" ref="K58">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B58,C58),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
       <c r="L58" s="12" t="str">
         <f t="array" ref="L58">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B58,C58),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+I</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="8">
-        <v>13.91</v>
+        <v>15.7</v>
       </c>
       <c r="C59" s="9">
-        <v>14.1</v>
+        <v>15.71</v>
       </c>
       <c r="D59" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="E59" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="F59" s="9" t="str">
-        <f t="array" ref="F59">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B59,C59),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F59">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B59,C59),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G59" s="9" t="str">
         <f t="array" ref="G59">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B59,C59),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+0</v>
       </c>
       <c r="H59" s="9" t="str">
         <f t="array" ref="H59">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B59,C59),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5135,39 +5144,39 @@
       </c>
       <c r="J59" s="9" t="str">
         <f t="array" ref="J59">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B59,C59),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K59" s="9" t="str">
         <f t="array" ref="K59">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B59,C59),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L59" s="12" t="str">
         <f t="array" ref="L59">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B59,C59),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="8">
-        <v>14.1</v>
+        <v>15.71</v>
       </c>
       <c r="C60" s="9">
-        <v>14.2</v>
+        <v>16</v>
       </c>
       <c r="D60" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="E60" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>+II</v>
+        <v>+0</v>
       </c>
       <c r="F60" s="9" t="str">
-        <f t="array" ref="F60">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B60,C60),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F60">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B60,C60),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G60" s="9" t="str">
         <f t="array" ref="G60">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B60,C60),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
+        <v>+0</v>
       </c>
       <c r="H60" s="9" t="str">
         <f t="array" ref="H60">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B60,C60),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5192,26 +5201,26 @@
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="8">
-        <v>14.2</v>
+        <v>16</v>
       </c>
       <c r="C61" s="9">
-        <v>14.21</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="D61" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E61" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F61" s="9" t="str">
-        <f t="array" ref="F61">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B61,C61),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F61">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B61,C61),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G61" s="9" t="str">
         <f t="array" ref="G61">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B61,C61),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="H61" s="9" t="str">
         <f t="array" ref="H61">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B61,C61),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5223,39 +5232,39 @@
       </c>
       <c r="J61" s="9" t="str">
         <f t="array" ref="J61">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B61,C61),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K61" s="9" t="str">
         <f t="array" ref="K61">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B61,C61),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L61" s="12" t="str">
         <f t="array" ref="L61">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B61,C61),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="8">
-        <v>14.21</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="C62" s="9">
-        <v>14.4</v>
+        <v>16.11</v>
       </c>
       <c r="D62" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E62" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F62" s="9" t="str">
-        <f t="array" ref="F62">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B62,C62),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F62">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B62,C62),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G62" s="9" t="str">
         <f t="array" ref="G62">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B62,C62),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="H62" s="9" t="str">
         <f t="array" ref="H62">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B62,C62),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5267,39 +5276,39 @@
       </c>
       <c r="J62" s="9" t="str">
         <f t="array" ref="J62">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B62,C62),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K62" s="9" t="str">
         <f t="array" ref="K62">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B62,C62),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L62" s="12" t="str">
         <f t="array" ref="L62">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B62,C62),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="8">
-        <v>14.4</v>
+        <v>16.11</v>
       </c>
       <c r="C63" s="9">
-        <v>14.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="D63" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E63" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F63" s="9" t="str">
-        <f t="array" ref="F63">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B63,C63),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
+        <f t="array" ref="F63">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B63,C63),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
         <v>+III</v>
       </c>
       <c r="G63" s="9" t="str">
         <f t="array" ref="G63">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B63,C63),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="H63" s="9" t="str">
         <f t="array" ref="H63">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B63,C63),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5324,26 +5333,26 @@
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
-        <v>14.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C64" s="9">
-        <v>14.799999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="D64" s="23" t="str">
         <f t="shared" si="2"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="E64" s="23" t="str">
         <f t="shared" si="3"/>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="F64" s="9" t="str">
-        <f t="array" ref="F64">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B64,C64),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F64">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B64,C64),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G64" s="9" t="str">
         <f t="array" ref="G64">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B64,C64),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-II</v>
+        <v>+0</v>
       </c>
       <c r="H64" s="9" t="str">
         <f t="array" ref="H64">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B64,C64),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5368,10 +5377,10 @@
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="8">
-        <v>14.799999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="C65" s="9">
-        <v>15</v>
+        <v>16.71</v>
       </c>
       <c r="D65" s="23" t="str">
         <f t="shared" si="2"/>
@@ -5382,8 +5391,8 @@
         <v>+0</v>
       </c>
       <c r="F65" s="9" t="str">
-        <f t="array" ref="F65">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B65,C65),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F65">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B65,C65),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G65" s="9" t="str">
         <f t="array" ref="G65">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B65,C65),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -5399,23 +5408,23 @@
       </c>
       <c r="J65" s="9" t="str">
         <f t="array" ref="J65">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B65,C65),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="K65" s="9" t="str">
         <f t="array" ref="K65">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B65,C65),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
       <c r="L65" s="12" t="str">
         <f t="array" ref="L65">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B65,C65),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
+        <v>+II</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="8">
-        <v>15</v>
+        <v>16.71</v>
       </c>
       <c r="C66" s="9">
-        <v>15.01</v>
+        <v>17.200000000000003</v>
       </c>
       <c r="D66" s="23" t="str">
         <f t="shared" si="2"/>
@@ -5426,8 +5435,8 @@
         <v>+0</v>
       </c>
       <c r="F66" s="9" t="str">
-        <f t="array" ref="F66">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B66,C66),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F66">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B66,C66),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G66" s="9" t="str">
         <f t="array" ref="G66">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B66,C66),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
@@ -5443,39 +5452,39 @@
       </c>
       <c r="J66" s="9" t="str">
         <f t="array" ref="J66">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B66,C66),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="K66" s="9" t="str">
         <f t="array" ref="K66">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B66,C66),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
       <c r="L66" s="12" t="str">
         <f t="array" ref="L66">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B66,C66),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
+        <v>NR</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="8">
-        <v>15.01</v>
+        <v>17.200000000000003</v>
       </c>
       <c r="C67" s="9">
-        <v>15.7</v>
+        <v>17.3</v>
       </c>
       <c r="D67" s="23" t="str">
-        <f t="shared" ref="D67:D82" si="4">IF(COUNTIF(F67:L67,"D")&gt;0,"D",IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR")))))))))</f>
-        <v>+0</v>
+        <f t="shared" ref="D67:D69" si="4">IF(COUNTIF(F67:L67,"D")&gt;0,"D",IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR")))))))))</f>
+        <v>-I</v>
       </c>
       <c r="E67" s="23" t="str">
-        <f t="shared" ref="E67:E82" si="5">IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR"))))))))</f>
-        <v>+0</v>
+        <f t="shared" ref="E67:E69" si="5">IF(COUNTIF(F67:L67,"-III")&gt;0,"-III",IF(COUNTIF(F67:L67,"-II")&gt;0,"-II",IF(COUNTIF(F67:L67,"-I")&gt;0,"-I",IF(COUNTIF(F67:L67,"+0")&gt;0,"+0",IF(COUNTIF(F67:L67,"+I")&gt;0,"+I",IF(COUNTIF(F67:L67,"+II")&gt;0,"+II",IF(COUNTIF(F67:L67,"+III")&gt;0,"+III",IF(COUNTIF(F67:L67,"ND")&gt;0,"ND","NR"))))))))</f>
+        <v>-I</v>
       </c>
       <c r="F67" s="9" t="str">
-        <f t="array" ref="F67">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B67,C67),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F67">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B67,C67),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G67" s="9" t="str">
         <f t="array" ref="G67">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B67,C67),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="H67" s="9" t="str">
         <f t="array" ref="H67">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B67,C67),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5500,26 +5509,26 @@
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="8">
-        <v>15.7</v>
+        <v>17.3</v>
       </c>
       <c r="C68" s="9">
-        <v>15.71</v>
+        <v>17.309999999999999</v>
       </c>
       <c r="D68" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="E68" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="F68" s="9" t="str">
-        <f t="array" ref="F68">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B68,C68),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F68">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B68,C68),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G68" s="9" t="str">
         <f t="array" ref="G68">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B68,C68),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="H68" s="9" t="str">
         <f t="array" ref="H68">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B68,C68),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5544,26 +5553,26 @@
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="8">
-        <v>15.71</v>
+        <v>17.309999999999999</v>
       </c>
       <c r="C69" s="9">
-        <v>16</v>
+        <v>17.5</v>
       </c>
       <c r="D69" s="23" t="str">
         <f t="shared" si="4"/>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="E69" s="23" t="str">
         <f t="shared" si="5"/>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="F69" s="9" t="str">
-        <f t="array" ref="F69">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B69,C69),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
+        <f t="array" ref="F69">INDEX(STPH!$O$11:$O$26,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$26&gt;AVERAGE(B69,C69),STPH!$D$11:$D$26)),STPH!$D$11:$D$26),1))</f>
+        <v>+I</v>
       </c>
       <c r="G69" s="9" t="str">
         <f t="array" ref="G69">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B69,C69),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
+        <v>-I</v>
       </c>
       <c r="H69" s="9" t="str">
         <f t="array" ref="H69">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B69,C69),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
@@ -5587,576 +5596,173 @@
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="8">
-        <v>16</v>
-      </c>
-      <c r="C70" s="9">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="D70" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E70" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F70" s="9" t="str">
-        <f t="array" ref="F70">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B70,C70),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G70" s="9" t="str">
-        <f t="array" ref="G70">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B70,C70),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H70" s="9" t="str">
-        <f t="array" ref="H70">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B70,C70),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I70" s="9" t="str">
-        <f t="array" ref="I70">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B70,C70),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J70" s="9" t="str">
-        <f t="array" ref="J70">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B70,C70),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K70" s="9" t="str">
-        <f t="array" ref="K70">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B70,C70),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L70" s="12" t="str">
-        <f t="array" ref="L70">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B70,C70),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="12"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="8">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C71" s="9">
-        <v>16.11</v>
-      </c>
-      <c r="D71" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E71" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F71" s="9" t="str">
-        <f t="array" ref="F71">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B71,C71),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G71" s="9" t="str">
-        <f t="array" ref="G71">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B71,C71),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H71" s="9" t="str">
-        <f t="array" ref="H71">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B71,C71),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I71" s="9" t="str">
-        <f t="array" ref="I71">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B71,C71),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J71" s="9" t="str">
-        <f t="array" ref="J71">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B71,C71),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="K71" s="9" t="str">
-        <f t="array" ref="K71">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B71,C71),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="L71" s="12" t="str">
-        <f t="array" ref="L71">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B71,C71),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
-      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="12"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B72" s="8">
-        <v>16.11</v>
-      </c>
-      <c r="C72" s="9">
-        <v>16.200000000000003</v>
-      </c>
-      <c r="D72" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E72" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F72" s="9" t="str">
-        <f t="array" ref="F72">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B72,C72),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G72" s="9" t="str">
-        <f t="array" ref="G72">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B72,C72),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H72" s="9" t="str">
-        <f t="array" ref="H72">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B72,C72),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I72" s="9" t="str">
-        <f t="array" ref="I72">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B72,C72),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J72" s="9" t="str">
-        <f t="array" ref="J72">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B72,C72),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K72" s="9" t="str">
-        <f t="array" ref="K72">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B72,C72),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L72" s="12" t="str">
-        <f t="array" ref="L72">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B72,C72),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="12"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B73" s="8">
-        <v>16.200000000000003</v>
-      </c>
-      <c r="C73" s="9">
-        <v>16.3</v>
-      </c>
-      <c r="D73" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E73" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F73" s="9" t="str">
-        <f t="array" ref="F73">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B73,C73),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G73" s="9" t="str">
-        <f t="array" ref="G73">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B73,C73),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H73" s="9" t="str">
-        <f t="array" ref="H73">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B73,C73),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I73" s="9" t="str">
-        <f t="array" ref="I73">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B73,C73),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J73" s="9" t="str">
-        <f t="array" ref="J73">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B73,C73),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K73" s="9" t="str">
-        <f t="array" ref="K73">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B73,C73),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L73" s="12" t="str">
-        <f t="array" ref="L73">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B73,C73),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="12"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B74" s="8">
-        <v>16.3</v>
-      </c>
-      <c r="C74" s="9">
-        <v>16.309999999999999</v>
-      </c>
-      <c r="D74" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E74" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F74" s="9" t="str">
-        <f t="array" ref="F74">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B74,C74),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G74" s="9" t="str">
-        <f t="array" ref="G74">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B74,C74),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H74" s="9" t="str">
-        <f t="array" ref="H74">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B74,C74),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I74" s="9" t="str">
-        <f t="array" ref="I74">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B74,C74),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J74" s="9" t="str">
-        <f t="array" ref="J74">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B74,C74),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K74" s="9" t="str">
-        <f t="array" ref="K74">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B74,C74),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L74" s="12" t="str">
-        <f t="array" ref="L74">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B74,C74),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="12"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="8">
-        <v>16.309999999999999</v>
-      </c>
-      <c r="C75" s="9">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="D75" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E75" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F75" s="9" t="str">
-        <f t="array" ref="F75">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B75,C75),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G75" s="9" t="str">
-        <f t="array" ref="G75">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B75,C75),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H75" s="9" t="str">
-        <f t="array" ref="H75">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B75,C75),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I75" s="9" t="str">
-        <f t="array" ref="I75">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B75,C75),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J75" s="9" t="str">
-        <f t="array" ref="J75">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B75,C75),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K75" s="9" t="str">
-        <f t="array" ref="K75">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B75,C75),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L75" s="12" t="str">
-        <f t="array" ref="L75">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B75,C75),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="12"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B76" s="8">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="C76" s="9">
-        <v>16.7</v>
-      </c>
-      <c r="D76" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E76" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F76" s="9" t="str">
-        <f t="array" ref="F76">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B76,C76),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G76" s="9" t="str">
-        <f t="array" ref="G76">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B76,C76),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H76" s="9" t="str">
-        <f t="array" ref="H76">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B76,C76),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I76" s="9" t="str">
-        <f t="array" ref="I76">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B76,C76),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J76" s="9" t="str">
-        <f t="array" ref="J76">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B76,C76),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K76" s="9" t="str">
-        <f t="array" ref="K76">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B76,C76),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L76" s="12" t="str">
-        <f t="array" ref="L76">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B76,C76),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B76" s="8"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="12"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="8">
-        <v>16.7</v>
-      </c>
-      <c r="C77" s="9">
-        <v>16.71</v>
-      </c>
-      <c r="D77" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E77" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F77" s="9" t="str">
-        <f t="array" ref="F77">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B77,C77),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G77" s="9" t="str">
-        <f t="array" ref="G77">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B77,C77),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H77" s="9" t="str">
-        <f t="array" ref="H77">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B77,C77),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I77" s="9" t="str">
-        <f t="array" ref="I77">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B77,C77),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J77" s="9" t="str">
-        <f t="array" ref="J77">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B77,C77),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="K77" s="9" t="str">
-        <f t="array" ref="K77">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B77,C77),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="L77" s="12" t="str">
-        <f t="array" ref="L77">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B77,C77),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
-      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="12"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B78" s="8">
-        <v>16.71</v>
-      </c>
-      <c r="C78" s="9">
-        <v>17.2</v>
-      </c>
-      <c r="D78" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>+0</v>
-      </c>
-      <c r="E78" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>+0</v>
-      </c>
-      <c r="F78" s="9" t="str">
-        <f t="array" ref="F78">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B78,C78),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G78" s="9" t="str">
-        <f t="array" ref="G78">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B78,C78),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+0</v>
-      </c>
-      <c r="H78" s="9" t="str">
-        <f t="array" ref="H78">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B78,C78),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I78" s="9" t="str">
-        <f t="array" ref="I78">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B78,C78),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J78" s="9" t="str">
-        <f t="array" ref="J78">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B78,C78),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K78" s="9" t="str">
-        <f t="array" ref="K78">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B78,C78),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L78" s="12" t="str">
-        <f t="array" ref="L78">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B78,C78),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B78" s="8"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="12"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B79" s="8">
-        <v>17.2</v>
-      </c>
-      <c r="C79" s="9">
-        <v>17.21</v>
-      </c>
-      <c r="D79" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>-I</v>
-      </c>
-      <c r="E79" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="F79" s="9" t="str">
-        <f t="array" ref="F79">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B79,C79),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G79" s="9" t="str">
-        <f t="array" ref="G79">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B79,C79),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-I</v>
-      </c>
-      <c r="H79" s="9" t="str">
-        <f t="array" ref="H79">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B79,C79),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I79" s="9" t="str">
-        <f t="array" ref="I79">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B79,C79),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J79" s="9" t="str">
-        <f t="array" ref="J79">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B79,C79),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K79" s="9" t="str">
-        <f t="array" ref="K79">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B79,C79),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L79" s="12" t="str">
-        <f t="array" ref="L79">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B79,C79),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="12"/>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B80" s="8">
-        <v>17.21</v>
-      </c>
-      <c r="C80" s="9">
-        <v>17.3</v>
-      </c>
-      <c r="D80" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>-I</v>
-      </c>
-      <c r="E80" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="F80" s="9" t="str">
-        <f t="array" ref="F80">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B80,C80),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G80" s="9" t="str">
-        <f t="array" ref="G80">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B80,C80),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-I</v>
-      </c>
-      <c r="H80" s="9" t="str">
-        <f t="array" ref="H80">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B80,C80),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I80" s="9" t="str">
-        <f t="array" ref="I80">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B80,C80),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J80" s="9" t="str">
-        <f t="array" ref="J80">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B80,C80),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K80" s="9" t="str">
-        <f t="array" ref="K80">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B80,C80),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L80" s="12" t="str">
-        <f t="array" ref="L80">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B80,C80),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="12"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B81" s="8">
-        <v>17.3</v>
-      </c>
-      <c r="C81" s="9">
-        <v>17.309999999999999</v>
-      </c>
-      <c r="D81" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>-I</v>
-      </c>
-      <c r="E81" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="F81" s="9" t="str">
-        <f t="array" ref="F81">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B81,C81),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G81" s="9" t="str">
-        <f t="array" ref="G81">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B81,C81),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-I</v>
-      </c>
-      <c r="H81" s="9" t="str">
-        <f t="array" ref="H81">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B81,C81),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I81" s="9" t="str">
-        <f t="array" ref="I81">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B81,C81),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J81" s="9" t="str">
-        <f t="array" ref="J81">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B81,C81),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="K81" s="9" t="str">
-        <f t="array" ref="K81">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B81,C81),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="L81" s="12" t="str">
-        <f t="array" ref="L81">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B81,C81),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>+II</v>
-      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="12"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B82" s="8">
-        <v>17.309999999999999</v>
-      </c>
-      <c r="C82" s="9">
-        <v>17.5</v>
-      </c>
-      <c r="D82" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>-I</v>
-      </c>
-      <c r="E82" s="23" t="str">
-        <f t="shared" si="5"/>
-        <v>-I</v>
-      </c>
-      <c r="F82" s="9" t="str">
-        <f t="array" ref="F82">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B82,C82),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+I</v>
-      </c>
-      <c r="G82" s="9" t="str">
-        <f t="array" ref="G82">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B82,C82),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>-I</v>
-      </c>
-      <c r="H82" s="9" t="str">
-        <f t="array" ref="H82">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B82,C82),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="I82" s="9" t="str">
-        <f t="array" ref="I82">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B82,C82),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="J82" s="9" t="str">
-        <f t="array" ref="J82">INDEX(STKWp!$K$11:$K$62,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$62&gt;AVERAGE(B82,C82),STKWp!$D$11:$D$62)),STKWp!$D$11:$D$62),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="K82" s="9" t="str">
-        <f t="array" ref="K82">INDEX(BSKW!$K$11:$K$109,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$109&gt;AVERAGE(B82,C82),BSKW!$D$11:$D$109)),BSKW!$D$11:$D$109),1))</f>
-        <v>NR</v>
-      </c>
-      <c r="L82" s="12" t="str">
-        <f t="array" ref="L82">INDEX(HTKW!$K$11:$K$86,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$86&gt;AVERAGE(B82,C82),HTKW!$D$11:$D$86)),HTKW!$D$11:$D$86),1))</f>
-        <v>NR</v>
-      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="12"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="8"/>
@@ -6554,10 +6160,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49710E67-B736-4749-B620-06835F5DE469}">
-  <dimension ref="B2:Y37"/>
+  <dimension ref="B2:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6611,7 +6217,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="26">
-        <f>IFERROR(MIN(1-PRODUCT(Q11:Q36),MAX(S11:S36)),"GR")</f>
+        <f>IFERROR(MIN(1-PRODUCT(Q11:Q26),MAX(S11:S26)),"GR")</f>
         <v>2.3947398894430538E-4</v>
       </c>
       <c r="E5" s="1"/>
@@ -6621,7 +6227,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="26">
-        <f>MIN(1-PRODUCT(R11:R36),MAX(T11:T36))</f>
+        <f>MIN(1-PRODUCT(R11:R26),MAX(T11:T26))</f>
         <v>2.3947398894430538E-4</v>
       </c>
       <c r="M6" s="1"/>
@@ -6635,7 +6241,7 @@
         <v>37</v>
       </c>
       <c r="C7" s="17" t="str">
-        <f>IF(1-PRODUCT(R11:R36)&gt;MAX(T11:T36),"Ja","Nee")</f>
+        <f>IF(1-PRODUCT(R11:R28)&gt;MAX(T11:T28),"Ja","Nee")</f>
         <v>Nee</v>
       </c>
       <c r="Q7" s="1"/>
@@ -6646,46 +6252,46 @@
       </c>
     </row>
     <row r="10" spans="2:25" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="B10" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="K10" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="19" t="s">
+      <c r="M10" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="19" t="s">
+      <c r="N10" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="74" t="s">
         <v>19</v>
       </c>
       <c r="P10" s="2"/>
@@ -6760,36 +6366,37 @@
         <f t="shared" ref="O11:O26" si="2">IF(E11="Nee","NR",IF(ISNUMBER($M11),W11,IF($X11,"D","ND")))</f>
         <v>+I</v>
       </c>
-      <c r="Q11" s="31">
-        <f t="shared" ref="Q11" si="3">IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="29">
+        <f>IF(AND(F11="Geen faalkans",I11="Nee"),1,1-M11)</f>
         <v>0.99999416666666663</v>
       </c>
-      <c r="R11" s="10">
-        <f t="shared" ref="R11" si="4">IF(M11="-",1,Q11)</f>
+      <c r="R11" s="5">
+        <f t="shared" ref="R11" si="3">IF(M11="-",1,Q11)</f>
         <v>0.99999416666666663</v>
       </c>
-      <c r="S11" s="10">
-        <f t="shared" ref="S11" si="5">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
+      <c r="S11" s="5">
+        <f t="shared" ref="S11" si="4">IF(AND(F11="Geen faalkans",I11="Nee"),0,L11*$C$3)</f>
         <v>7.2250000000000008E-5</v>
       </c>
-      <c r="T11" s="10">
-        <f t="shared" ref="T11" si="6">IF(L11="-",0,S11)</f>
+      <c r="T11" s="5">
+        <f t="shared" ref="T11" si="5">IF(L11="-",0,S11)</f>
         <v>7.2250000000000008E-5</v>
       </c>
-      <c r="U11" s="9">
+      <c r="U11" s="4">
         <f t="array" ref="U11">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M11,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>3.3333333333333335E-5</v>
       </c>
-      <c r="V11" s="9">
+      <c r="V11" s="4">
         <f>IFERROR(MATCH($U11,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>3</v>
       </c>
-      <c r="W11" s="9" t="str">
+      <c r="W11" s="4" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,V11)</f>
         <v>+I</v>
       </c>
-      <c r="X11" s="12" t="b">
-        <f t="shared" ref="X11:X26" si="7">IF($E11="Ja",IF($I11="Ja",NOT(ISNUMBER($J11)),FALSE),FALSE)</f>
+      <c r="X11" s="7" t="b">
+        <f t="shared" ref="X11:X26" si="6">IF($E11="Ja",IF($I11="Ja",NOT(ISNUMBER($J11)),FALSE),FALSE)</f>
         <v>0</v>
       </c>
     </row>
@@ -6829,7 +6436,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M12" s="10">
-        <f t="shared" ref="M12:M26" si="8">IF($E12="Nee",0,IF(I12="Ja",IF(ISNUMBER(K12),K12,"-"),IF(ISNUMBER(H12),H12,"-")))</f>
+        <f t="shared" ref="M12:M26" si="7">IF($E12="Nee",0,IF(I12="Ja",IF(ISNUMBER(K12),K12,"-"),IF(ISNUMBER(H12),H12,"-")))</f>
         <v>4.8333333333333376E-6</v>
       </c>
       <c r="N12" s="11">
@@ -6840,20 +6447,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P12" s="9"/>
       <c r="Q12" s="31">
-        <f t="shared" ref="Q12:Q26" si="9">IF(AND(F12="Geen faalkans",I12="Nee"),1,1-M12)</f>
+        <f t="shared" ref="Q12:Q26" si="8">IF(AND(F12="Geen faalkans",I12="Nee"),1,1-M12)</f>
         <v>0.99999516666666666</v>
       </c>
       <c r="R12" s="10">
-        <f t="shared" ref="R12:R26" si="10">IF(M12="-",1,Q12)</f>
+        <f t="shared" ref="R12:R26" si="9">IF(M12="-",1,Q12)</f>
         <v>0.99999516666666666</v>
       </c>
       <c r="S12" s="10">
-        <f t="shared" ref="S12:S26" si="11">IF(AND(F12="Geen faalkans",I12="Nee"),0,L12*$C$3)</f>
+        <f t="shared" ref="S12:S26" si="10">IF(AND(F12="Geen faalkans",I12="Nee"),0,L12*$C$3)</f>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="T12" s="10">
-        <f t="shared" ref="T12:T26" si="12">IF(L12="-",0,S12)</f>
+        <f t="shared" ref="T12:T26" si="11">IF(L12="-",0,S12)</f>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U12" s="9">
@@ -6869,7 +6477,7 @@
         <v>+I</v>
       </c>
       <c r="X12" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -6909,7 +6517,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M13" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>5.1666666666666632E-6</v>
       </c>
       <c r="N13" s="11">
@@ -6920,20 +6528,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P13" s="9"/>
       <c r="Q13" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999483333333339</v>
+      </c>
+      <c r="R13" s="10">
         <f t="shared" si="9"/>
         <v>0.99999483333333339</v>
       </c>
-      <c r="R13" s="10">
+      <c r="S13" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999483333333339</v>
-      </c>
-      <c r="S13" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T13" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T13" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U13" s="9">
@@ -6949,7 +6558,7 @@
         <v>+I</v>
       </c>
       <c r="X13" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -6985,7 +6594,7 @@
         <v>5.4514800000000002E-5</v>
       </c>
       <c r="M14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.7808168000000009E-4</v>
       </c>
       <c r="N14" s="11">
@@ -6996,20 +6605,21 @@
         <f t="shared" si="2"/>
         <v>+0</v>
       </c>
+      <c r="P14" s="9"/>
       <c r="Q14" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99982191832</v>
+      </c>
+      <c r="R14" s="10">
         <f t="shared" si="9"/>
         <v>0.99982191832</v>
       </c>
-      <c r="R14" s="10">
+      <c r="S14" s="10">
         <f t="shared" si="10"/>
-        <v>0.99982191832</v>
-      </c>
-      <c r="S14" s="10">
+        <v>1.57547772E-3</v>
+      </c>
+      <c r="T14" s="10">
         <f t="shared" si="11"/>
-        <v>1.57547772E-3</v>
-      </c>
-      <c r="T14" s="10">
-        <f t="shared" si="12"/>
         <v>1.57547772E-3</v>
       </c>
       <c r="U14" s="9">
@@ -7025,7 +6635,7 @@
         <v>+0</v>
       </c>
       <c r="X14" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7065,7 +6675,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M15" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.6666666666666657E-6</v>
       </c>
       <c r="N15" s="11">
@@ -7076,20 +6686,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P15" s="9"/>
       <c r="Q15" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999633333333338</v>
+      </c>
+      <c r="R15" s="10">
         <f t="shared" si="9"/>
         <v>0.99999633333333338</v>
       </c>
-      <c r="R15" s="10">
+      <c r="S15" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999633333333338</v>
-      </c>
-      <c r="S15" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T15" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T15" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U15" s="9">
@@ -7105,7 +6716,7 @@
         <v>+I</v>
       </c>
       <c r="X15" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7145,7 +6756,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M16" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.0000000000000013E-6</v>
       </c>
       <c r="N16" s="11">
@@ -7156,20 +6767,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P16" s="9"/>
       <c r="Q16" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999199999999999</v>
+      </c>
+      <c r="R16" s="10">
         <f t="shared" si="9"/>
         <v>0.99999199999999999</v>
       </c>
-      <c r="R16" s="10">
+      <c r="S16" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999199999999999</v>
-      </c>
-      <c r="S16" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T16" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T16" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U16" s="9">
@@ -7185,7 +6797,7 @@
         <v>+I</v>
       </c>
       <c r="X16" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7221,7 +6833,7 @@
         <v>2.2578500000000001E-13</v>
       </c>
       <c r="M17" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.9672699999999963E-13</v>
       </c>
       <c r="N17" s="11">
@@ -7232,20 +6844,21 @@
         <f t="shared" si="2"/>
         <v>+III</v>
       </c>
+      <c r="P17" s="9"/>
       <c r="Q17" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999999999950329</v>
+      </c>
+      <c r="R17" s="10">
         <f t="shared" si="9"/>
         <v>0.99999999999950329</v>
       </c>
-      <c r="R17" s="10">
+      <c r="S17" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999999999950329</v>
-      </c>
-      <c r="S17" s="10">
+        <v>6.5251865E-12</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="11"/>
-        <v>6.5251865E-12</v>
-      </c>
-      <c r="T17" s="10">
-        <f t="shared" si="12"/>
         <v>6.5251865E-12</v>
       </c>
       <c r="U17" s="9">
@@ -7261,7 +6874,7 @@
         <v>+III</v>
       </c>
       <c r="X17" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7297,7 +6910,7 @@
         <v>4.2707099999999999E-13</v>
       </c>
       <c r="M18" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>5.6942799999999998E-13</v>
       </c>
       <c r="N18" s="11">
@@ -7308,20 +6921,21 @@
         <f t="shared" si="2"/>
         <v>+III</v>
       </c>
+      <c r="P18" s="9"/>
       <c r="Q18" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999999999943057</v>
+      </c>
+      <c r="R18" s="10">
         <f t="shared" si="9"/>
         <v>0.99999999999943057</v>
       </c>
-      <c r="R18" s="10">
+      <c r="S18" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999999999943057</v>
-      </c>
-      <c r="S18" s="10">
+        <v>1.2342351899999998E-11</v>
+      </c>
+      <c r="T18" s="10">
         <f t="shared" si="11"/>
-        <v>1.2342351899999998E-11</v>
-      </c>
-      <c r="T18" s="10">
-        <f t="shared" si="12"/>
         <v>1.2342351899999998E-11</v>
       </c>
       <c r="U18" s="9">
@@ -7337,7 +6951,7 @@
         <v>+III</v>
       </c>
       <c r="X18" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7377,7 +6991,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.6666666666666717E-6</v>
       </c>
       <c r="N19" s="11">
@@ -7388,20 +7002,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P19" s="9"/>
       <c r="Q19" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999633333333338</v>
+      </c>
+      <c r="R19" s="10">
         <f t="shared" si="9"/>
         <v>0.99999633333333338</v>
       </c>
-      <c r="R19" s="10">
+      <c r="S19" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999633333333338</v>
-      </c>
-      <c r="S19" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T19" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T19" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U19" s="9">
@@ -7417,7 +7032,7 @@
         <v>+I</v>
       </c>
       <c r="X19" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7457,7 +7072,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>8.1666666666666641E-6</v>
       </c>
       <c r="N20" s="11">
@@ -7468,20 +7083,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P20" s="9"/>
       <c r="Q20" s="31">
+        <f t="shared" si="8"/>
+        <v>0.9999918333333333</v>
+      </c>
+      <c r="R20" s="10">
         <f t="shared" si="9"/>
         <v>0.9999918333333333</v>
       </c>
-      <c r="R20" s="10">
+      <c r="S20" s="10">
         <f t="shared" si="10"/>
-        <v>0.9999918333333333</v>
-      </c>
-      <c r="S20" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T20" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T20" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U20" s="9">
@@ -7497,7 +7113,7 @@
         <v>+I</v>
       </c>
       <c r="X20" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7537,7 +7153,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M21" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.8333333333333308E-6</v>
       </c>
       <c r="N21" s="11">
@@ -7548,20 +7164,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P21" s="9"/>
       <c r="Q21" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999516666666666</v>
+      </c>
+      <c r="R21" s="10">
         <f t="shared" si="9"/>
         <v>0.99999516666666666</v>
       </c>
-      <c r="R21" s="10">
+      <c r="S21" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999516666666666</v>
-      </c>
-      <c r="S21" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T21" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T21" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U21" s="9">
@@ -7577,7 +7194,7 @@
         <v>+I</v>
       </c>
       <c r="X21" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7617,7 +7234,7 @@
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="M22" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>9.5000000000000056E-6</v>
       </c>
       <c r="N22" s="11">
@@ -7628,20 +7245,21 @@
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
+      <c r="P22" s="9"/>
       <c r="Q22" s="31">
+        <f t="shared" si="8"/>
+        <v>0.9999905</v>
+      </c>
+      <c r="R22" s="10">
         <f t="shared" si="9"/>
         <v>0.9999905</v>
       </c>
-      <c r="R22" s="10">
+      <c r="S22" s="10">
         <f t="shared" si="10"/>
-        <v>0.9999905</v>
-      </c>
-      <c r="S22" s="10">
+        <v>7.2250000000000008E-5</v>
+      </c>
+      <c r="T22" s="10">
         <f t="shared" si="11"/>
-        <v>7.2250000000000008E-5</v>
-      </c>
-      <c r="T22" s="10">
-        <f t="shared" si="12"/>
         <v>7.2250000000000008E-5</v>
       </c>
       <c r="U22" s="9">
@@ -7657,7 +7275,7 @@
         <v>+I</v>
       </c>
       <c r="X22" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7693,7 +7311,7 @@
         <v>6.3678600000000002E-8</v>
       </c>
       <c r="M23" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>2.5046915999999996E-7</v>
       </c>
       <c r="N23" s="11">
@@ -7704,20 +7322,21 @@
         <f t="shared" si="2"/>
         <v>+III</v>
       </c>
+      <c r="P23" s="9"/>
       <c r="Q23" s="31">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="R23" s="10">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="R23" s="10">
+      <c r="S23" s="10">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="S23" s="10">
+        <v>0</v>
+      </c>
+      <c r="T23" s="10">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="10">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="U23" s="9">
@@ -7733,7 +7352,7 @@
         <v>+III</v>
       </c>
       <c r="X23" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7769,7 +7388,7 @@
         <v>5.6538300000000003E-8</v>
       </c>
       <c r="M24" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.7715333999999999E-7</v>
       </c>
       <c r="N24" s="11">
@@ -7780,20 +7399,21 @@
         <f t="shared" si="2"/>
         <v>+III</v>
       </c>
+      <c r="P24" s="9"/>
       <c r="Q24" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999982284666</v>
+      </c>
+      <c r="R24" s="10">
         <f t="shared" si="9"/>
         <v>0.99999982284666</v>
       </c>
-      <c r="R24" s="10">
+      <c r="S24" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999982284666</v>
-      </c>
-      <c r="S24" s="10">
+        <v>1.63395687E-6</v>
+      </c>
+      <c r="T24" s="10">
         <f t="shared" si="11"/>
-        <v>1.63395687E-6</v>
-      </c>
-      <c r="T24" s="10">
-        <f t="shared" si="12"/>
         <v>1.63395687E-6</v>
       </c>
       <c r="U24" s="9">
@@ -7809,7 +7429,7 @@
         <v>+III</v>
       </c>
       <c r="X24" s="12" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -7845,7 +7465,7 @@
         <v>1.0956199999999999E-12</v>
       </c>
       <c r="M25" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.6799999999999999E-12</v>
       </c>
       <c r="N25" s="11">
@@ -7856,20 +7476,21 @@
         <f t="shared" si="2"/>
         <v>+III</v>
       </c>
+      <c r="P25" s="9"/>
       <c r="Q25" s="31">
+        <f t="shared" si="8"/>
+        <v>0.99999999999832001</v>
+      </c>
+      <c r="R25" s="10">
         <f t="shared" si="9"/>
         <v>0.99999999999832001</v>
       </c>
-      <c r="R25" s="10">
+      <c r="S25" s="10">
         <f t="shared" si="10"/>
-        <v>0.99999999999832001</v>
-      </c>
-      <c r="S25" s="10">
+        <v>3.1663417999999999E-11</v>
+      </c>
+      <c r="T25" s="10">
         <f t="shared" si="11"/>
-        <v>3.1663417999999999E-11</v>
-      </c>
-      <c r="T25" s="10">
-        <f t="shared" si="12"/>
         <v>3.1663417999999999E-11</v>
       </c>
       <c r="U25" s="9">
@@ -7885,300 +7506,105 @@
         <v>+III</v>
       </c>
       <c r="X25" s="12" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="14">
         <v>16.399999999999999</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="14">
         <v>17.5</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="15">
         <v>3.0666800000000001E-6</v>
       </c>
-      <c r="H26" s="26">
+      <c r="H26" s="27">
         <v>7.5611000000000003E-6</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="10"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="31">
+      <c r="I26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="33">
         <f t="shared" si="0"/>
         <v>3.0666800000000001E-6</v>
       </c>
-      <c r="M26" s="10">
-        <f t="shared" si="8"/>
+      <c r="M26" s="15">
+        <f t="shared" si="7"/>
         <v>7.5611000000000003E-6</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="16">
         <f t="shared" si="1"/>
         <v>2.4655653671070996</v>
       </c>
-      <c r="O26" s="32" t="str">
+      <c r="O26" s="34" t="str">
         <f t="shared" si="2"/>
         <v>+I</v>
       </c>
-      <c r="Q26" s="31">
+      <c r="P26" s="14"/>
+      <c r="Q26" s="33">
+        <f t="shared" si="8"/>
+        <v>0.9999924389</v>
+      </c>
+      <c r="R26" s="15">
         <f t="shared" si="9"/>
         <v>0.9999924389</v>
       </c>
-      <c r="R26" s="10">
+      <c r="S26" s="15">
         <f t="shared" si="10"/>
-        <v>0.9999924389</v>
-      </c>
-      <c r="S26" s="10">
+        <v>8.8627051999999999E-5</v>
+      </c>
+      <c r="T26" s="15">
         <f t="shared" si="11"/>
         <v>8.8627051999999999E-5</v>
       </c>
-      <c r="T26" s="10">
-        <f t="shared" si="12"/>
-        <v>8.8627051999999999E-5</v>
-      </c>
-      <c r="U26" s="9">
+      <c r="U26" s="14">
         <f t="array" ref="U26">MIN(IF('Normen en duidingsklassen'!$E$13:$E$20&gt;=$M26,'Normen en duidingsklassen'!$E$13:$E$20))</f>
         <v>3.3333333333333335E-5</v>
       </c>
-      <c r="V26" s="9">
+      <c r="V26" s="14">
         <f>IFERROR(MATCH($U26,'Normen en duidingsklassen'!$E$13:$E$20,0),1)</f>
         <v>3</v>
       </c>
-      <c r="W26" s="9" t="str">
+      <c r="W26" s="14" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$13:$D$20,V26)</f>
         <v>+I</v>
       </c>
-      <c r="X26" s="12" t="b">
-        <f t="shared" si="7"/>
+      <c r="X26" s="17" t="b">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="31"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="32"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="12"/>
+      <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="32"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
-      <c r="W28" s="9"/>
-      <c r="X28" s="12"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="32"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="12"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="32"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="12"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="32"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
-      <c r="T31" s="10"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="12"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="32"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="10"/>
-      <c r="S32" s="10"/>
-      <c r="T32" s="10"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="12"/>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="32"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="12"/>
-    </row>
-    <row r="34" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="13"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="34"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
-      <c r="U34" s="14"/>
-      <c r="V34" s="14"/>
-      <c r="W34" s="14"/>
-      <c r="X34" s="17"/>
-    </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="O37" t="s">
-        <v>174</v>
-      </c>
+      <c r="Q28" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G11:H34">
+  <conditionalFormatting sqref="G11:H26">
     <cfRule type="expression" dxfId="107" priority="11">
       <formula>IF($E11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:K34">
+  <conditionalFormatting sqref="J11:K26">
     <cfRule type="expression" dxfId="106" priority="10">
       <formula>IF($I11="Nee",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O11:O34">
+  <conditionalFormatting sqref="O11:O26">
     <cfRule type="cellIs" dxfId="105" priority="1" operator="equal">
       <formula>"0"</formula>
     </cfRule>
@@ -8261,7 +7687,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>O11:O34</xm:sqref>
+          <xm:sqref>O11:O26</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -8271,7 +7697,7 @@
           <x14:formula1>
             <xm:f>Informatiepagina!$B$15:$B$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E35:E50 F11:F34</xm:sqref>
+          <xm:sqref>E27:E42 F11:F26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8284,7 +7710,7 @@
   <dimension ref="B2:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D11" sqref="D11:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10186,7 +9612,7 @@
   <dimension ref="B2:U73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="D11" sqref="D11:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12729,8 +12155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4337BDE-5D5C-4814-877A-41AF49DBDF5F}">
   <dimension ref="B2:U62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T12" sqref="M12:T57"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15956,7 +15382,7 @@
   <dimension ref="B2:U109"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="T12" sqref="M12:T57"/>
+      <selection activeCell="D11" sqref="D11:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20211,8 +19637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A27DBF-2298-4509-84AE-DCEFED147711}">
   <dimension ref="B2:U85"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="T12" sqref="M12:T57"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D57" sqref="D11:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>